<commit_message>
setting for Powersafe changed and some fixes for Mega-sketch
</commit_message>
<xml_diff>
--- a/PIN_assignment_arduino.xlsx
+++ b/PIN_assignment_arduino.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\gesichert\GitHub\honigautomat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40154E18-2396-4241-9425-7336D4CC5F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AC05D8-B91D-4773-A5CB-F03C4B9D2589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29925" yWindow="1290" windowWidth="24690" windowHeight="11385" activeTab="1" xr2:uid="{1A94CFE8-7D10-41CB-9C3C-AAF15650CB36}"/>
+    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{1A94CFE8-7D10-41CB-9C3C-AAF15650CB36}"/>
   </bookViews>
   <sheets>
     <sheet name="Mega 2560" sheetId="1" r:id="rId1"/>
@@ -799,10 +799,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3389049-E811-4D4F-9E84-6B31736A3147}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,7 +1483,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="31" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1489,7 +1492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B258A34D-C685-424C-BBF8-04F539479062}">
   <dimension ref="B2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
coin acceptor can be disabled; bill payment, credit cards
it is now possible to disable the coin acceptor when all products are sold out.
Payment with bill (Geldscheinleser) NV10 now possible.
Cashless payment (e.g. Creditcard, Debitcard, Applepay ...) now supported
</commit_message>
<xml_diff>
--- a/PIN_assignment_arduino.xlsx
+++ b/PIN_assignment_arduino.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\gesichert\GitHub\honigautomat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD92B52-B722-4ADA-8F02-440F8233A6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32B2329-B805-4500-9572-AF7EC030C52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A94CFE8-7D10-41CB-9C3C-AAF15650CB36}"/>
+    <workbookView xWindow="30435" yWindow="0" windowWidth="24690" windowHeight="13890" xr2:uid="{1A94CFE8-7D10-41CB-9C3C-AAF15650CB36}"/>
   </bookViews>
   <sheets>
     <sheet name="Mega 2560" sheetId="1" r:id="rId1"/>
@@ -21,19 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="95">
   <si>
     <t>PIN</t>
   </si>
@@ -298,6 +291,28 @@
   </si>
   <si>
     <t>for smarthome system e.g. homematic (inform about a sold item)</t>
+  </si>
+  <si>
+    <t>cashless payment onyx</t>
+  </si>
+  <si>
+    <t>coin power</t>
+  </si>
+  <si>
+    <t>coin acceptor power - allows to turn off coin acceptor when all compartments are
+empty</t>
+  </si>
+  <si>
+    <t>NV10 bill reader</t>
+  </si>
+  <si>
+    <t>nv 10 channel 1 open</t>
+  </si>
+  <si>
+    <t>nv 10 channel 2 open</t>
+  </si>
+  <si>
+    <t>onyx inhibit</t>
   </si>
 </sst>
 </file>
@@ -414,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -445,6 +460,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -474,7 +492,7 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>637188</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>18192</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -800,7 +818,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -813,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,16 +946,25 @@
       <c r="B11">
         <v>9</v>
       </c>
+      <c r="E11" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>10</v>
       </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>11</v>
       </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -964,19 +991,37 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>18</v>
       </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
coin acceptor can be disabled; bill payement ; kreditcards
it is now possible to disable the coin acceptor when all products are sold out.
Payment with bill (Geldscheinleser) NV10 now possible.
Cashless payment (e.g. Creditcard, Debitcard, Applepay ...) now supported
</commit_message>
<xml_diff>
--- a/PIN_assignment_arduino.xlsx
+++ b/PIN_assignment_arduino.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\gesichert\GitHub\honigautomat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD92B52-B722-4ADA-8F02-440F8233A6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32B2329-B805-4500-9572-AF7EC030C52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A94CFE8-7D10-41CB-9C3C-AAF15650CB36}"/>
+    <workbookView xWindow="30435" yWindow="0" windowWidth="24690" windowHeight="13890" xr2:uid="{1A94CFE8-7D10-41CB-9C3C-AAF15650CB36}"/>
   </bookViews>
   <sheets>
     <sheet name="Mega 2560" sheetId="1" r:id="rId1"/>
@@ -21,19 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="95">
   <si>
     <t>PIN</t>
   </si>
@@ -298,6 +291,28 @@
   </si>
   <si>
     <t>for smarthome system e.g. homematic (inform about a sold item)</t>
+  </si>
+  <si>
+    <t>cashless payment onyx</t>
+  </si>
+  <si>
+    <t>coin power</t>
+  </si>
+  <si>
+    <t>coin acceptor power - allows to turn off coin acceptor when all compartments are
+empty</t>
+  </si>
+  <si>
+    <t>NV10 bill reader</t>
+  </si>
+  <si>
+    <t>nv 10 channel 1 open</t>
+  </si>
+  <si>
+    <t>nv 10 channel 2 open</t>
+  </si>
+  <si>
+    <t>onyx inhibit</t>
   </si>
 </sst>
 </file>
@@ -414,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -445,6 +460,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -474,7 +492,7 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>637188</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>18192</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -800,7 +818,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -813,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,16 +946,25 @@
       <c r="B11">
         <v>9</v>
       </c>
+      <c r="E11" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>10</v>
       </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>11</v>
       </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -964,19 +991,37 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>18</v>
       </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
r3 bill payment and cooling
bill payment for Mega
cooling with DS18B20 for UNO
</commit_message>
<xml_diff>
--- a/PIN_assignment_arduino.xlsx
+++ b/PIN_assignment_arduino.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\gesichert\GitHub\honigautomat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\gesichert\github\honigautomat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32B2329-B805-4500-9572-AF7EC030C52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45526BB7-7939-4F44-9636-DF1AE6A42AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30435" yWindow="0" windowWidth="24690" windowHeight="13890" xr2:uid="{1A94CFE8-7D10-41CB-9C3C-AAF15650CB36}"/>
+    <workbookView xWindow="32640" yWindow="1755" windowWidth="24270" windowHeight="17145" xr2:uid="{1A94CFE8-7D10-41CB-9C3C-AAF15650CB36}"/>
   </bookViews>
   <sheets>
     <sheet name="Mega 2560" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="103">
   <si>
     <t>PIN</t>
   </si>
@@ -223,9 +223,6 @@
     <t>selector [4]</t>
   </si>
   <si>
-    <t>empty or for smarthome system e.g. homematic (inform about a sold item)</t>
-  </si>
-  <si>
     <t>Coin acceptor(at the coin acceptor: use COIN, not count! Set switch to "FAST" )</t>
   </si>
   <si>
@@ -238,12 +235,6 @@
     <t>Button 5</t>
   </si>
   <si>
-    <t>row 1</t>
-  </si>
-  <si>
-    <t>row 2</t>
-  </si>
-  <si>
     <t>setup button</t>
   </si>
   <si>
@@ -263,12 +254,6 @@
   </si>
   <si>
     <t>config / setup button</t>
-  </si>
-  <si>
-    <t>powersave</t>
-  </si>
-  <si>
-    <t>powersave 2nd option</t>
   </si>
   <si>
     <t>alternative assignement
@@ -313,6 +298,45 @@
   </si>
   <si>
     <t>onyx inhibit</t>
+  </si>
+  <si>
+    <t>-5V</t>
+  </si>
+  <si>
+    <t>Sommerbetrieb (gegen -5V setzen)</t>
+  </si>
+  <si>
+    <t>tempsensor</t>
+  </si>
+  <si>
+    <t>cooling relais</t>
+  </si>
+  <si>
+    <t>powersave relais</t>
+  </si>
+  <si>
+    <t>Temperature sensor DS18B20</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>connect to pin "tempsensor" and via 4.7k ohm resistor with +5V</t>
+  </si>
+  <si>
+    <t>+5V</t>
+  </si>
+  <si>
+    <t>GND (5V)</t>
+  </si>
+  <si>
+    <t>activate NV10: connect to GND</t>
+  </si>
+  <si>
+    <t>activate bill payment: connect to GND</t>
   </si>
 </sst>
 </file>
@@ -349,7 +373,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,6 +440,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -429,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -463,6 +499,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -818,7 +857,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -832,7 +871,7 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +888,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -865,7 +904,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -879,7 +918,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
         <v>38</v>
@@ -921,7 +960,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>30</v>
@@ -947,7 +986,7 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -955,7 +994,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -963,18 +1002,24 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>12</v>
       </c>
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>13</v>
       </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -996,10 +1041,10 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1010,7 +1055,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -1021,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -1359,7 +1404,7 @@
         <v>52</v>
       </c>
       <c r="E54" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F54" t="s">
         <v>38</v>
@@ -1370,7 +1415,7 @@
         <v>53</v>
       </c>
       <c r="E55" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
@@ -1553,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B258A34D-C685-424C-BBF8-04F539479062}">
-  <dimension ref="B2:H22"/>
+  <dimension ref="B2:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,14 +1619,14 @@
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>82</v>
+        <v>76</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -1589,13 +1634,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
         <v>68</v>
       </c>
-      <c r="E3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>33</v>
+      <c r="F3" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -1605,12 +1650,6 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -1620,10 +1659,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -1631,16 +1667,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
         <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1648,16 +1678,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
         <v>40</v>
-      </c>
-      <c r="F7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -1665,16 +1689,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
         <v>41</v>
-      </c>
-      <c r="F8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -1682,16 +1700,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
         <v>42</v>
-      </c>
-      <c r="F9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -1699,16 +1711,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
         <v>43</v>
-      </c>
-      <c r="F10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -1716,16 +1722,13 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>34</v>
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -1733,16 +1736,10 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>25</v>
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1750,16 +1747,10 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>31</v>
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -1767,19 +1758,10 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>32</v>
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -1787,19 +1769,13 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>33</v>
+      <c r="F15" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1807,10 +1783,13 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1824,10 +1803,10 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>32</v>
+        <v>70</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1841,10 +1820,10 @@
         <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>31</v>
+        <v>71</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1858,10 +1837,10 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>25</v>
+        <v>72</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1875,10 +1854,10 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>34</v>
+        <v>73</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1889,7 +1868,7 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>29</v>
@@ -1903,10 +1882,39 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H22" s="21" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E27" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E28" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/matgrhn/honigautomat"
This reverts commit 5830dfdff19be9e6b2ad839832d81a4e94c98684, reversing
changes made to 5e11ea68bec77137a8a4cc21740d7d277648e682.
</commit_message>
<xml_diff>
--- a/PIN_assignment_arduino.xlsx
+++ b/PIN_assignment_arduino.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\gesichert\GitHub\honigautomat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\gesichert\github\honigautomat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32B2329-B805-4500-9572-AF7EC030C52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45526BB7-7939-4F44-9636-DF1AE6A42AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30435" yWindow="0" windowWidth="24690" windowHeight="13890" xr2:uid="{1A94CFE8-7D10-41CB-9C3C-AAF15650CB36}"/>
+    <workbookView xWindow="32640" yWindow="1755" windowWidth="24270" windowHeight="17145" xr2:uid="{1A94CFE8-7D10-41CB-9C3C-AAF15650CB36}"/>
   </bookViews>
   <sheets>
     <sheet name="Mega 2560" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="103">
   <si>
     <t>PIN</t>
   </si>
@@ -223,9 +223,6 @@
     <t>selector [4]</t>
   </si>
   <si>
-    <t>empty or for smarthome system e.g. homematic (inform about a sold item)</t>
-  </si>
-  <si>
     <t>Coin acceptor(at the coin acceptor: use COIN, not count! Set switch to "FAST" )</t>
   </si>
   <si>
@@ -238,12 +235,6 @@
     <t>Button 5</t>
   </si>
   <si>
-    <t>row 1</t>
-  </si>
-  <si>
-    <t>row 2</t>
-  </si>
-  <si>
     <t>setup button</t>
   </si>
   <si>
@@ -263,12 +254,6 @@
   </si>
   <si>
     <t>config / setup button</t>
-  </si>
-  <si>
-    <t>powersave</t>
-  </si>
-  <si>
-    <t>powersave 2nd option</t>
   </si>
   <si>
     <t>alternative assignement
@@ -313,6 +298,45 @@
   </si>
   <si>
     <t>onyx inhibit</t>
+  </si>
+  <si>
+    <t>-5V</t>
+  </si>
+  <si>
+    <t>Sommerbetrieb (gegen -5V setzen)</t>
+  </si>
+  <si>
+    <t>tempsensor</t>
+  </si>
+  <si>
+    <t>cooling relais</t>
+  </si>
+  <si>
+    <t>powersave relais</t>
+  </si>
+  <si>
+    <t>Temperature sensor DS18B20</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>connect to pin "tempsensor" and via 4.7k ohm resistor with +5V</t>
+  </si>
+  <si>
+    <t>+5V</t>
+  </si>
+  <si>
+    <t>GND (5V)</t>
+  </si>
+  <si>
+    <t>activate NV10: connect to GND</t>
+  </si>
+  <si>
+    <t>activate bill payment: connect to GND</t>
   </si>
 </sst>
 </file>
@@ -349,7 +373,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,6 +440,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -429,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -463,6 +499,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -818,7 +857,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -832,7 +871,7 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +888,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -865,7 +904,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -879,7 +918,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
         <v>38</v>
@@ -921,7 +960,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>30</v>
@@ -947,7 +986,7 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -955,7 +994,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -963,18 +1002,24 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>12</v>
       </c>
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>13</v>
       </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -996,10 +1041,10 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1010,7 +1055,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -1021,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -1359,7 +1404,7 @@
         <v>52</v>
       </c>
       <c r="E54" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F54" t="s">
         <v>38</v>
@@ -1370,7 +1415,7 @@
         <v>53</v>
       </c>
       <c r="E55" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
@@ -1553,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B258A34D-C685-424C-BBF8-04F539479062}">
-  <dimension ref="B2:H22"/>
+  <dimension ref="B2:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,14 +1619,14 @@
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>82</v>
+        <v>76</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -1589,13 +1634,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
         <v>68</v>
       </c>
-      <c r="E3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>33</v>
+      <c r="F3" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -1605,12 +1650,6 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -1620,10 +1659,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -1631,16 +1667,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
         <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1648,16 +1678,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
         <v>40</v>
-      </c>
-      <c r="F7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -1665,16 +1689,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
         <v>41</v>
-      </c>
-      <c r="F8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -1682,16 +1700,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
         <v>42</v>
-      </c>
-      <c r="F9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -1699,16 +1711,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
         <v>43</v>
-      </c>
-      <c r="F10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -1716,16 +1722,13 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>34</v>
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -1733,16 +1736,10 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>25</v>
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1750,16 +1747,10 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>31</v>
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -1767,19 +1758,10 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>32</v>
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -1787,19 +1769,13 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>33</v>
+      <c r="F15" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1807,10 +1783,13 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1824,10 +1803,10 @@
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>32</v>
+        <v>70</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1841,10 +1820,10 @@
         <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>31</v>
+        <v>71</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1858,10 +1837,10 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>25</v>
+        <v>72</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1875,10 +1854,10 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>34</v>
+        <v>73</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1889,7 +1868,7 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>29</v>
@@ -1903,10 +1882,39 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H22" s="21" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E27" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E28" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SIM800L SMS & Paypal
now possible to send and receive SMS, can be used to configure threshold (receive) on which number of remaining products sms to be send. In addition to load money onto the system and payment with Paypal
</commit_message>
<xml_diff>
--- a/PIN_assignment_arduino.xlsx
+++ b/PIN_assignment_arduino.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\gesichert\github\honigautomat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45526BB7-7939-4F44-9636-DF1AE6A42AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952E6A25-5B17-4727-B239-C5704EB0D43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32640" yWindow="1755" windowWidth="24270" windowHeight="17145" xr2:uid="{1A94CFE8-7D10-41CB-9C3C-AAF15650CB36}"/>
+    <workbookView xWindow="2535" yWindow="600" windowWidth="24945" windowHeight="21180" xr2:uid="{1A94CFE8-7D10-41CB-9C3C-AAF15650CB36}"/>
   </bookViews>
   <sheets>
     <sheet name="Mega 2560" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="108">
   <si>
     <t>PIN</t>
   </si>
@@ -269,19 +269,10 @@
     <t>SCL  I2C port Display</t>
   </si>
   <si>
-    <t>Open Box - if electronical lock is implemented</t>
-  </si>
-  <si>
     <t xml:space="preserve">empty </t>
   </si>
   <si>
-    <t>for smarthome system e.g. homematic (inform about a sold item)</t>
-  </si>
-  <si>
     <t>cashless payment onyx</t>
-  </si>
-  <si>
-    <t>coin power</t>
   </si>
   <si>
     <t>coin acceptor power - allows to turn off coin acceptor when all compartments are
@@ -337,6 +328,31 @@
   </si>
   <si>
     <t>activate bill payment: connect to GND</t>
+  </si>
+  <si>
+    <t>smarthome info about sold items</t>
+  </si>
+  <si>
+    <t>smarthome</t>
+  </si>
+  <si>
+    <t>coin power
+ relais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sim 800L SMS module </t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>RX</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>Buzzer to inform about incoming Paypal money transfer</t>
   </si>
 </sst>
 </file>
@@ -870,8 +886,8 @@
   </sheetPr>
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +920,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -970,6 +986,12 @@
       <c r="B8">
         <v>6</v>
       </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -986,7 +1008,7 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -994,7 +1016,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1002,7 +1024,7 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1010,7 +1032,7 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1018,7 +1040,7 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1040,11 +1062,11 @@
       <c r="B19">
         <v>17</v>
       </c>
-      <c r="C19" t="s">
-        <v>84</v>
+      <c r="C19" s="22" t="s">
+        <v>102</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1055,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -1066,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -1376,9 +1398,13 @@
       <c r="B51">
         <v>49</v>
       </c>
-      <c r="C51" s="12"/>
+      <c r="C51" t="s">
+        <v>106</v>
+      </c>
       <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
+      <c r="E51" t="s">
+        <v>107</v>
+      </c>
       <c r="F51" s="12"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
@@ -1398,24 +1424,27 @@
       <c r="B53">
         <v>51</v>
       </c>
+      <c r="C53" t="s">
+        <v>104</v>
+      </c>
+      <c r="E53" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>52</v>
       </c>
-      <c r="E54" t="s">
-        <v>80</v>
-      </c>
-      <c r="F54" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>53</v>
       </c>
+      <c r="C55" t="s">
+        <v>105</v>
+      </c>
       <c r="E55" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
@@ -1640,7 +1669,7 @@
         <v>68</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -1725,10 +1754,10 @@
         <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -1739,7 +1768,7 @@
         <v>67</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1750,7 +1779,7 @@
         <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -1761,7 +1790,7 @@
         <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -1775,7 +1804,7 @@
         <v>26</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1789,7 +1818,7 @@
         <v>69</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1806,7 +1835,7 @@
         <v>70</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1823,7 +1852,7 @@
         <v>71</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1840,7 +1869,7 @@
         <v>72</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1857,7 +1886,7 @@
         <v>73</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1890,28 +1919,28 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E27" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E28" s="23" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E29" s="23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>29</v>

</xml_diff>